<commit_message>
Added a new spreadsheet (.xlsx and .csv) to file that includes sites and their distance upstream and their larger drainage basin areas
</commit_message>
<xml_diff>
--- a/site_DATAexplore/SUMPpnts_distArea_final.xlsx
+++ b/site_DATAexplore/SUMPpnts_distArea_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamjohnson/Desktop/Laura/Hallett_Lab/Repositories/thesis-mussels/site_DATAexplore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42605ED8-D7A6-F54B-AC5F-93CB950AD44B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C19141-827C-2F4F-850E-2E2A978468A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9100" yWindow="1040" windowWidth="28140" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28140" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mussel_aggs" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="103">
   <si>
     <t>obs_id</t>
   </si>
@@ -284,13 +284,73 @@
   </si>
   <si>
     <t>tiller</t>
+  </si>
+  <si>
+    <t>site_id</t>
+  </si>
+  <si>
+    <t>BKY01</t>
+  </si>
+  <si>
+    <t>BKY02</t>
+  </si>
+  <si>
+    <t>BKY03</t>
+  </si>
+  <si>
+    <t>BKY04</t>
+  </si>
+  <si>
+    <t>BKY05</t>
+  </si>
+  <si>
+    <t>CNYNPK</t>
+  </si>
+  <si>
+    <t>TIL02</t>
+  </si>
+  <si>
+    <t>TIL03</t>
+  </si>
+  <si>
+    <t>DAYSCH</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>OB</t>
+  </si>
+  <si>
+    <t>ZINCCMP</t>
+  </si>
+  <si>
+    <t>COW01</t>
+  </si>
+  <si>
+    <t>COW02</t>
+  </si>
+  <si>
+    <t>MAFA_DaysChute</t>
+  </si>
+  <si>
+    <t>MAFA_CoffeCr</t>
+  </si>
+  <si>
+    <t>MAFA_HappyValley</t>
+  </si>
+  <si>
+    <t>MAFA_OB</t>
+  </si>
+  <si>
+    <t>MAFA_SR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +362,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -324,9 +390,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,1425 +674,1628 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1">
+        <v>84</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1">
         <v>65053.320862562447</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>65.053320862562444</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>40.422247037691292</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="2">
         <v>1430</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1">
+        <v>84</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
         <v>65386.106462587391</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>65.386106462587392</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>40.629030358764389</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="2">
         <v>1430</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1">
+        <v>84</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1">
         <v>65155.440712581913</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>65.155440712581907</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>40.485701351017738</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="2">
         <v>1430</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1">
+        <v>85</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1">
         <v>71337.08325869996</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>71.337083258699963</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>44.326794761541656</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1">
+        <v>86</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
         <v>73836.541067645783</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>73.836541067645783</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>45.879885359744129</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1">
+        <v>86</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1">
         <v>73897.394259949302</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>73.897394259949309</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>45.917697768698957</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1">
+        <v>86</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1">
         <v>74277.680100462705</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>74.277680100462703</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>46.153996361704614</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1">
+        <v>86</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
         <v>74539.012304531381</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>74.539012304531383</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>46.31638061467897</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1">
+        <v>87</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1">
         <v>78498.541026495222</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>78.498541026495218</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>48.776716936174367</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1">
+        <v>87</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1">
         <v>78715.650297680608</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>78.715650297680611</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>48.911622341120101</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1">
+        <v>87</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1">
         <v>78854.833245320828</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>78.854833245320833</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>48.998106588478251</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1">
+        <v>87</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1">
         <v>79007.850963154604</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>79.00785096315461</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>49.093187360826342</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="1">
+        <v>88</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1">
         <v>97223.84</v>
       </c>
-      <c r="D14" s="1">
-        <f>C14/1000</f>
+      <c r="E14" s="1">
+        <f>D14/1000</f>
         <v>97.223839999999996</v>
       </c>
-      <c r="E14" s="1">
-        <f>D14/1.609</f>
+      <c r="F14" s="1">
+        <f>E14/1.609</f>
         <v>60.425009322560598</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="2">
         <v>1270</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1">
+        <v>88</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1">
         <v>97382.55</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" ref="D15:D21" si="0">C15/1000</f>
+      <c r="E15" s="1">
+        <f t="shared" ref="E15:E21" si="0">D15/1000</f>
         <v>97.382550000000009</v>
       </c>
-      <c r="E15" s="1">
-        <f t="shared" ref="E15:E21" si="1">D15/1.609</f>
+      <c r="F15" s="1">
+        <f t="shared" ref="F15:F21" si="1">E15/1.609</f>
         <v>60.52364822871349</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="2">
         <v>1270</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1">
+        <v>88</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1">
         <v>97523.1</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <f t="shared" si="0"/>
         <v>97.523099999999999</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <f t="shared" si="1"/>
         <v>60.61100062150404</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="2">
         <v>1270</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1">
+        <v>88</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1">
         <v>97400.573999999993</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>97.400573999999992</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <f t="shared" si="1"/>
         <v>60.534850217526412</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="2">
         <v>1270</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="1">
+        <v>88</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1">
         <v>97517</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <f t="shared" si="0"/>
         <v>97.516999999999996</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <f t="shared" si="1"/>
         <v>60.607209446861404</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="2">
         <v>1270</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="1">
+        <v>88</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1">
         <v>96752.054000000004</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <f t="shared" si="0"/>
         <v>96.752054000000001</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <f t="shared" si="1"/>
         <v>60.131792417650715</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="2">
         <v>1270</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="1">
+        <v>88</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1">
         <v>96752.282000000007</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>96.752282000000008</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <f t="shared" si="1"/>
         <v>60.131934120571792</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="2">
         <v>1270</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="1">
+        <v>88</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="1">
         <v>96940.631999999998</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <f t="shared" si="0"/>
         <v>96.940631999999994</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <f t="shared" si="1"/>
         <v>60.248994406463638</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="2">
         <v>1270</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="1">
+        <v>89</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1">
         <v>113672.701</v>
       </c>
-      <c r="D22" s="1">
-        <f>C22/1000</f>
+      <c r="E22" s="1">
+        <f>D22/1000</f>
         <v>113.672701</v>
       </c>
-      <c r="E22" s="1">
-        <f>D22/1.609</f>
+      <c r="F22" s="1">
+        <f>E22/1.609</f>
         <v>70.648042883778743</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="2">
         <v>699</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="1">
+        <v>89</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="1">
         <v>113765.942</v>
       </c>
-      <c r="D23" s="1">
-        <f t="shared" ref="D23:D27" si="2">C23/1000</f>
+      <c r="E23" s="1">
+        <f t="shared" ref="E23:E27" si="2">D23/1000</f>
         <v>113.765942</v>
       </c>
-      <c r="E23" s="1">
-        <f t="shared" ref="E23:E27" si="3">D23/1.609</f>
+      <c r="F23" s="1">
+        <f t="shared" ref="F23:F27" si="3">E23/1.609</f>
         <v>70.705992541951517</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="2">
         <v>699</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="1">
+        <v>89</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1">
         <v>113785.09</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <f t="shared" si="2"/>
         <v>113.78509</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <f t="shared" si="3"/>
         <v>70.717893101305151</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="2">
         <v>699</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="1">
+        <v>89</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1">
         <v>113800.6</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <f t="shared" si="2"/>
         <v>113.8006</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <f t="shared" si="3"/>
         <v>70.727532628962095</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="2">
         <v>699</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="1">
+        <v>89</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1">
         <v>113800.394</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <f t="shared" si="2"/>
         <v>113.800394</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <f t="shared" si="3"/>
         <v>70.727404599129898</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="2">
         <v>699</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="1">
+        <v>89</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1">
         <v>113849.914</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <f t="shared" si="2"/>
         <v>113.849914</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <f t="shared" si="3"/>
         <v>70.758181479179612</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="2">
         <v>699</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="1">
+        <v>90</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="1">
         <v>152572.38714233448</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>152.57238714233449</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>94.804056771019518</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="2">
         <v>571</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="1">
+        <v>90</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="1">
         <v>152439.50110931747</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>152.43950110931746</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>94.721485243797702</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="2">
         <v>571</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="1">
+        <v>91</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="1">
         <v>158755.18619946545</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>158.75518619946544</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>98.645868803948048</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="2">
         <v>564</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="1">
+        <v>91</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1">
         <v>158624.18827399999</v>
       </c>
-      <c r="D31" s="1">
-        <f>C31/1000</f>
+      <c r="E31" s="1">
+        <f>D31/1000</f>
         <v>158.62418827399998</v>
       </c>
-      <c r="E31" s="1">
-        <f>D31*0.621371</f>
+      <c r="F31" s="1">
+        <f>E31*0.621371</f>
         <v>98.564470492003636</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="2">
         <v>564</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="1">
+        <v>92</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="1">
         <v>129912.24</v>
       </c>
-      <c r="D32" s="1">
-        <f>C32/1000</f>
+      <c r="E32" s="1">
+        <f>D32/1000</f>
         <v>129.91224</v>
       </c>
-      <c r="E32" s="1">
-        <f>D32/1.609</f>
+      <c r="F32" s="1">
+        <f>E32/1.609</f>
         <v>80.740981976382841</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="2">
         <v>643</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="1">
+        <v>92</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="1">
         <v>129960.838</v>
       </c>
-      <c r="D33" s="1">
-        <f t="shared" ref="D33:D47" si="4">C33/1000</f>
+      <c r="E33" s="1">
+        <f t="shared" ref="E33:E47" si="4">D33/1000</f>
         <v>129.960838</v>
       </c>
-      <c r="E33" s="1">
-        <f t="shared" ref="E33:E47" si="5">D33/1.609</f>
+      <c r="F33" s="1">
+        <f t="shared" ref="F33:F47" si="5">E33/1.609</f>
         <v>80.771185829707889</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="2">
         <v>643</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="1">
+        <v>92</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="1">
         <v>129942.77099999999</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <f t="shared" si="4"/>
         <v>129.94277099999999</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <f t="shared" si="5"/>
         <v>80.759957116221258</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="2">
         <v>643</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="1">
+        <v>92</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="1">
         <v>129995.481</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="1">
         <f t="shared" si="4"/>
         <v>129.99548100000001</v>
       </c>
-      <c r="E35" s="1">
+      <c r="F35" s="1">
         <f t="shared" si="5"/>
         <v>80.792716594157866</v>
       </c>
-      <c r="F35" s="1">
+      <c r="G35" s="2">
         <v>643</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" s="1">
+        <v>92</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="1">
         <v>130182.427</v>
       </c>
-      <c r="D36" s="1">
+      <c r="E36" s="1">
         <f t="shared" si="4"/>
         <v>130.18242699999999</v>
       </c>
-      <c r="E36" s="1">
+      <c r="F36" s="1">
         <f t="shared" si="5"/>
         <v>80.908904288377869</v>
       </c>
-      <c r="F36" s="1">
+      <c r="G36" s="2">
         <v>643</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="1">
+        <v>92</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="1">
         <v>130316.891</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <f t="shared" si="4"/>
         <v>130.316891</v>
       </c>
-      <c r="E37" s="1">
+      <c r="F37" s="1">
         <f t="shared" si="5"/>
         <v>80.992474207582347</v>
       </c>
-      <c r="F37" s="1">
+      <c r="G37" s="2">
         <v>643</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="1">
+        <v>92</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="1">
         <v>130128.48699999999</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <f t="shared" si="4"/>
         <v>130.12848700000001</v>
       </c>
-      <c r="E38" s="1">
+      <c r="F38" s="1">
         <f t="shared" si="5"/>
         <v>80.875380360472349</v>
       </c>
-      <c r="F38" s="1">
+      <c r="G38" s="2">
         <v>643</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" s="1">
+        <v>92</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="1">
         <v>130094.93</v>
       </c>
-      <c r="D39" s="1">
+      <c r="E39" s="1">
         <f t="shared" si="4"/>
         <v>130.09493000000001</v>
       </c>
-      <c r="E39" s="1">
+      <c r="F39" s="1">
         <f t="shared" si="5"/>
         <v>80.854524549409575</v>
       </c>
-      <c r="F39" s="1">
+      <c r="G39" s="2">
         <v>643</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="1">
+        <v>93</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="1">
         <v>157348.109</v>
       </c>
-      <c r="D40" s="1">
+      <c r="E40" s="1">
         <f t="shared" si="4"/>
         <v>157.34810899999999</v>
       </c>
-      <c r="E40" s="1">
+      <c r="F40" s="1">
         <f t="shared" si="5"/>
         <v>97.79248539465506</v>
       </c>
-      <c r="F40" s="1">
+      <c r="G40" s="2">
         <v>565</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="1">
+        <v>93</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="1">
         <v>157580.96599999999</v>
       </c>
-      <c r="D41" s="1">
+      <c r="E41" s="1">
         <f t="shared" si="4"/>
         <v>157.58096599999999</v>
       </c>
-      <c r="E41" s="1">
+      <c r="F41" s="1">
         <f t="shared" si="5"/>
         <v>97.937206960845245</v>
       </c>
-      <c r="F41" s="1">
+      <c r="G41" s="2">
         <v>565</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" s="1">
+        <v>94</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1">
         <v>159871.80499999999</v>
       </c>
-      <c r="D42" s="1">
+      <c r="E42" s="1">
         <f t="shared" si="4"/>
         <v>159.87180499999999</v>
       </c>
-      <c r="E42" s="1">
+      <c r="F42" s="1">
         <f t="shared" si="5"/>
         <v>99.360972653822245</v>
       </c>
-      <c r="F42" s="1">
+      <c r="G42" s="2">
         <v>545</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" s="1">
+        <v>94</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="1">
         <v>159945.03599999999</v>
       </c>
-      <c r="D43" s="1">
+      <c r="E43" s="1">
         <f t="shared" si="4"/>
         <v>159.94503599999999</v>
       </c>
-      <c r="E43" s="1">
+      <c r="F43" s="1">
         <f t="shared" si="5"/>
         <v>99.406486016159093</v>
       </c>
-      <c r="F43" s="1">
+      <c r="G43" s="2">
         <v>545</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C44" s="1">
+        <v>94</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="1">
         <v>159984.503</v>
       </c>
-      <c r="D44" s="1">
+      <c r="E44" s="1">
         <f t="shared" si="4"/>
         <v>159.98450299999999</v>
       </c>
-      <c r="E44" s="1">
+      <c r="F44" s="1">
         <f t="shared" si="5"/>
         <v>99.431014916096956</v>
       </c>
-      <c r="F44" s="1">
+      <c r="G44" s="2">
         <v>545</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C45" s="1">
+        <v>94</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="1">
         <v>160109.67300000001</v>
       </c>
-      <c r="D45" s="1">
+      <c r="E45" s="1">
         <f t="shared" si="4"/>
         <v>160.10967300000002</v>
       </c>
-      <c r="E45" s="1">
+      <c r="F45" s="1">
         <f t="shared" si="5"/>
         <v>99.508808576755754</v>
       </c>
-      <c r="F45" s="1">
+      <c r="G45" s="2">
         <v>545</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" s="1">
+        <v>95</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="1">
         <v>196288.24299999999</v>
       </c>
-      <c r="D46" s="1">
+      <c r="E46" s="1">
         <f t="shared" si="4"/>
         <v>196.28824299999999</v>
       </c>
-      <c r="E46" s="1">
+      <c r="F46" s="1">
         <f t="shared" si="5"/>
         <v>121.99393598508389</v>
       </c>
-      <c r="F46" s="1">
+      <c r="G46" s="2">
         <v>193</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" s="1">
+        <v>95</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="1">
         <v>196196.88800000001</v>
       </c>
-      <c r="D47" s="1">
+      <c r="E47" s="1">
         <f t="shared" si="4"/>
         <v>196.196888</v>
       </c>
-      <c r="E47" s="1">
+      <c r="F47" s="1">
         <f t="shared" si="5"/>
         <v>121.93715848353014</v>
       </c>
-      <c r="F47" s="1">
+      <c r="G47" s="2">
         <v>193</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C48" s="1">
+        <v>22</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="1">
         <v>79066.503306887185</v>
       </c>
-      <c r="D48" s="1">
+      <c r="E48" s="1">
         <v>79.066503306887185</v>
       </c>
-      <c r="E48" s="1">
+      <c r="F48" s="1">
         <v>49.129632226303798</v>
       </c>
-      <c r="F48" s="1">
+      <c r="G48" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C49" s="1">
+        <v>23</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="1">
         <v>113879.44178389855</v>
       </c>
-      <c r="D49" s="1">
+      <c r="E49" s="1">
         <v>113.87944178389856</v>
       </c>
-      <c r="E49" s="1">
+      <c r="F49" s="1">
         <v>70.761382620702832</v>
       </c>
-      <c r="F49" s="1">
+      <c r="G49" s="2">
         <v>699</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C50" s="1">
+        <v>99</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="1">
         <v>158490.60965393484</v>
       </c>
-      <c r="D50" s="1">
+      <c r="E50" s="1">
         <v>158.49060965393485</v>
       </c>
-      <c r="E50" s="1">
+      <c r="F50" s="1">
         <v>98.481468611275147</v>
       </c>
-      <c r="F50" s="1">
+      <c r="G50" s="2">
         <v>564</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C51" s="1">
+        <v>98</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="1">
         <v>129974.94981455638</v>
       </c>
-      <c r="D51" s="1">
+      <c r="E51" s="1">
         <v>129.9749498145564</v>
       </c>
-      <c r="E51" s="1">
+      <c r="F51" s="1">
         <v>80.762664541220715</v>
       </c>
-      <c r="F51" s="1">
+      <c r="G51" s="2">
         <v>643</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C52" s="1">
+        <v>98</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="1">
         <v>129974.94981455638</v>
       </c>
-      <c r="D52" s="1">
+      <c r="E52" s="1">
         <v>129.9749498145564</v>
       </c>
-      <c r="E52" s="1">
+      <c r="F52" s="1">
         <v>80.762664541220715</v>
       </c>
-      <c r="F52" s="1">
+      <c r="G52" s="2">
         <v>643</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C53" s="1">
+        <v>27</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="1">
         <v>137669.01243141145</v>
       </c>
-      <c r="D53" s="1">
+      <c r="E53" s="1">
         <v>137.66901243141146</v>
       </c>
-      <c r="E53" s="1">
+      <c r="F53" s="1">
         <v>85.543531923518572</v>
       </c>
-      <c r="F53" s="1">
+      <c r="G53" s="2">
         <v>630</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C54" s="1">
+        <v>100</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="1">
         <v>39247.526389932493</v>
       </c>
-      <c r="D54" s="1">
+      <c r="E54" s="1">
         <v>39.247526389932496</v>
       </c>
-      <c r="E54" s="1">
+      <c r="F54" s="1">
         <v>24.387274720438743</v>
       </c>
-      <c r="F54" s="1">
+      <c r="G54" s="2">
         <v>1640</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C55" s="1">
+        <v>100</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="1">
         <v>39235.953918583808</v>
       </c>
-      <c r="D55" s="1">
+      <c r="E55" s="1">
         <v>39.23595391858381</v>
       </c>
-      <c r="E55" s="1">
+      <c r="F55" s="1">
         <v>24.38008392234434</v>
       </c>
-      <c r="F55" s="1">
+      <c r="G55" s="2">
         <v>1640</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C56" s="1">
+        <v>30</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="1">
         <v>73793.71406355458</v>
       </c>
-      <c r="D56" s="1">
+      <c r="E56" s="1">
         <v>73.793714063554589</v>
       </c>
-      <c r="E56" s="1">
+      <c r="F56" s="1">
         <v>45.853273901384973</v>
       </c>
-      <c r="F56" s="1">
+      <c r="G56" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C57" s="1">
+        <v>101</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="1">
         <v>160095.24817083243</v>
       </c>
-      <c r="D57" s="1">
+      <c r="E57" s="1">
         <v>160.09524817083243</v>
       </c>
-      <c r="E57" s="1">
+      <c r="F57" s="1">
         <v>99.478544451158328</v>
       </c>
-      <c r="F57" s="1">
+      <c r="G57" s="2">
         <v>545</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C58" s="1">
+        <v>101</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="1">
         <v>159827.60795750958</v>
       </c>
-      <c r="D58" s="1">
+      <c r="E58" s="1">
         <v>159.82760795750957</v>
       </c>
-      <c r="E58" s="1">
+      <c r="F58" s="1">
         <v>99.312240584165693</v>
       </c>
-      <c r="F58" s="1">
+      <c r="G58" s="2">
         <v>545</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C59" s="1">
+        <v>33</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="1">
         <v>166877.09780876833</v>
       </c>
-      <c r="D59" s="1">
+      <c r="E59" s="1">
         <v>166.87709780876833</v>
       </c>
-      <c r="E59" s="1">
+      <c r="F59" s="1">
         <v>103.69258914253219</v>
       </c>
-      <c r="F59" s="1">
+      <c r="G59" s="2">
         <v>451</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C60" s="1">
+        <v>102</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="1">
         <v>157435.97869809557</v>
       </c>
-      <c r="D60" s="1">
+      <c r="E60" s="1">
         <v>157.43597869809557</v>
       </c>
-      <c r="E60" s="1">
+      <c r="F60" s="1">
         <v>97.826151519614342</v>
       </c>
-      <c r="F60" s="1">
+      <c r="G60" s="2">
         <v>565</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C61" s="1">
+        <v>35</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="1">
         <v>173265.32358764537</v>
       </c>
-      <c r="D61" s="1">
+      <c r="E61" s="1">
         <v>173.26532358764538</v>
       </c>
-      <c r="E61" s="1">
+      <c r="F61" s="1">
         <v>107.6620473829788</v>
       </c>
-      <c r="F61" s="1">
+      <c r="G61" s="2">
         <v>441</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="A62" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C62" s="1">
+        <v>36</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="1">
         <v>70924.440120825282</v>
       </c>
-      <c r="D62" s="1">
+      <c r="E62" s="1">
         <v>70.924440120825281</v>
       </c>
-      <c r="E62" s="1">
+      <c r="F62" s="1">
         <v>44.070390282317327</v>
       </c>
-      <c r="F62" s="1">
+      <c r="G62" s="2">
         <v>1410</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="A63" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C63" s="1">
+      <c r="D63" s="1">
         <v>36468.024718883717</v>
       </c>
-      <c r="D63" s="1">
+      <c r="E63" s="1">
         <v>36.468024718883719</v>
       </c>
-      <c r="E63" s="1">
+      <c r="F63" s="1">
         <v>22.660172987597495</v>
       </c>
-      <c r="F63" s="1">
+      <c r="G63" s="2">
         <v>474</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="A64" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C64" s="1">
+      <c r="D64" s="1">
         <v>36618.387372952697</v>
       </c>
-      <c r="D64" s="1">
+      <c r="E64" s="1">
         <v>36.618387372952697</v>
       </c>
-      <c r="E64" s="1">
+      <c r="F64" s="1">
         <v>22.753603980318992</v>
       </c>
-      <c r="F64" s="1">
+      <c r="G64" s="2">
         <v>474</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C65" s="1">
+      <c r="D65" s="1">
         <v>37054.80273783172</v>
       </c>
-      <c r="D65" s="1">
+      <c r="E65" s="1">
         <v>37.054802737831722</v>
       </c>
-      <c r="E65" s="1">
+      <c r="F65" s="1">
         <v>23.024779832009234</v>
       </c>
-      <c r="F65" s="1">
+      <c r="G65" s="2">
         <v>474</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C66" s="1">
+      <c r="D66" s="1">
         <v>36322.368584171185</v>
       </c>
-      <c r="D66" s="1">
+      <c r="E66" s="1">
         <v>36.322368584171187</v>
       </c>
-      <c r="E66" s="1">
+      <c r="F66" s="1">
         <v>22.569666489515033</v>
       </c>
-      <c r="F66" s="1">
+      <c r="G66" s="2">
         <v>474</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7">
       <c r="A67" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C67" s="1">
+      <c r="D67" s="1">
         <v>45843.168603325073</v>
       </c>
-      <c r="D67" s="1">
+      <c r="E67" s="1">
         <v>45.843168603325076</v>
       </c>
-      <c r="E67" s="1">
+      <c r="F67" s="1">
         <v>28.485615518216704</v>
       </c>
-      <c r="F67" s="1">
+      <c r="G67" s="2">
         <v>394</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2038,9 +2308,9 @@
       <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -2054,7 +2324,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -2070,7 +2340,7 @@
         <v>28.841463020509632</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -2099,12 +2369,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2112,7 +2382,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2120,7 +2390,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2128,7 +2398,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2136,7 +2406,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2144,7 +2414,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>43</v>
       </c>

</xml_diff>